<commit_message>
EPBDS-9427 Fix NPE in RulesFrontend proxy
</commit_message>
<xml_diff>
--- a/WSFrontend/org.openl.rules.ruleservice/test-resources/RulesFrontendTest/multimodule/Module3_1.xlsx
+++ b/WSFrontend/org.openl.rules.ruleservice/test-resources/RulesFrontendTest/multimodule/Module3_1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\WSFrontend\org.openl.rules.ruleservice\test-resources\RulesFrontendTest\multimodule\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD90D145-0A10-424B-B7B0-626CE1F8AE1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19035" windowHeight="10995"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Environment</t>
   </si>
@@ -56,13 +62,19 @@
   </si>
   <si>
     <t>return "World, " + baseHello(hour) + "!";</t>
+  </si>
+  <si>
+    <t>return "i: " + I +" s: " + s;</t>
+  </si>
+  <si>
+    <t>Method String worldHello(Integer i, String s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,11 +165,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Vehicle-Eligibility"/>
@@ -253,7 +273,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,9 +305,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,6 +357,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -494,77 +550,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C12"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -572,7 +625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
@@ -580,17 +633,31 @@
         <v>5</v>
       </c>
     </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
+  <mergeCells count="11">
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>